<commit_message>
First-solo flight today! 🥳
</commit_message>
<xml_diff>
--- a/log/My_Flying_Logbook.xlsx
+++ b/log/My_Flying_Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haoren/Documents/PA28/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606A3CC9-CEEE-9A43-AFE4-4D7D5ED7A948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE5D0DF-68AD-5C49-A30D-56AE6E0EC574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{634C8D91-949A-EA46-A557-4B6714D72E97}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
   <si>
     <t>Month</t>
   </si>
@@ -197,15 +197,9 @@
     <t>R. Brown</t>
   </si>
   <si>
-    <t>Stamped</t>
-  </si>
-  <si>
     <t>Circuits Check</t>
   </si>
   <si>
-    <t>Page 1</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
@@ -213,6 +207,21 @@
   </si>
   <si>
     <t>TOTALS TO DATE</t>
+  </si>
+  <si>
+    <t>First Solo Flight</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>First Solo Stamped</t>
+  </si>
+  <si>
+    <t>Time Check Stamped</t>
+  </si>
+  <si>
+    <t>Page 1 END</t>
   </si>
 </sst>
 </file>
@@ -224,7 +233,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,13 +260,25 @@
       <name val="Courier"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -352,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,31 +465,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -787,10 +835,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -806,112 +854,113 @@
     <col min="13" max="26" width="5.7109375" style="8" customWidth="1"/>
     <col min="27" max="28" width="9.7109375" style="8" customWidth="1"/>
     <col min="29" max="29" width="12.42578125" style="7"/>
-    <col min="30" max="32" width="17.7109375" style="7" customWidth="1"/>
+    <col min="30" max="30" width="19.7109375" style="7" customWidth="1"/>
+    <col min="31" max="32" width="17.7109375" style="7" customWidth="1"/>
     <col min="33" max="16384" width="12.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="31" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="35" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="36"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="33" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33" t="s">
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="33" t="s">
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="33"/>
+      <c r="AB1" s="32"/>
       <c r="AD1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" s="28" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="2" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="33" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33" t="s">
+      <c r="N2" s="32"/>
+      <c r="O2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33" t="s">
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33" t="s">
+      <c r="R2" s="32"/>
+      <c r="S2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33" t="s">
+      <c r="T2" s="32"/>
+      <c r="U2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33" t="s">
+      <c r="V2" s="32"/>
+      <c r="W2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33" t="s">
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33" t="s">
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="33" t="s">
+      <c r="AB2" s="32" t="s">
         <v>19</v>
       </c>
     </row>
@@ -928,8 +977,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
@@ -939,9 +988,9 @@
       <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
@@ -984,8 +1033,8 @@
       <c r="Z3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
     </row>
     <row r="4" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1019,21 +1068,21 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="N4" s="43"/>
       <c r="O4" s="5">
         <v>0.8</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="43"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
+      <c r="R4" s="43"/>
       <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="T4" s="43"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
+      <c r="V4" s="43"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
+      <c r="X4" s="43"/>
       <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="Z4" s="43"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
     </row>
@@ -1067,21 +1116,21 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="44"/>
       <c r="O5" s="1">
         <v>1</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="44"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="R5" s="44"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="T5" s="44"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
+      <c r="V5" s="44"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
+      <c r="X5" s="44"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Z5" s="44"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
@@ -1115,21 +1164,21 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="N6" s="44"/>
       <c r="O6" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="44"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="44"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="44"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
+      <c r="V6" s="44"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
+      <c r="X6" s="44"/>
       <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="Z6" s="44"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
     </row>
@@ -1163,21 +1212,21 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="N7" s="44"/>
       <c r="O7" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="44"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+      <c r="R7" s="44"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
+      <c r="T7" s="44"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
+      <c r="V7" s="44"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
+      <c r="X7" s="44"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="Z7" s="44"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
     </row>
@@ -1211,21 +1260,21 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="44"/>
       <c r="O8" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="44"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="44"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="T8" s="44"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
+      <c r="V8" s="44"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+      <c r="X8" s="44"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="44"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
     </row>
@@ -1261,21 +1310,21 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="44"/>
       <c r="O9" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="44"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="R9" s="44"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="T9" s="44"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="V9" s="44"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
+      <c r="X9" s="44"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="44"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
     </row>
@@ -1309,21 +1358,21 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="44"/>
       <c r="O10" s="1">
         <v>1.3</v>
       </c>
-      <c r="P10" s="1"/>
+      <c r="P10" s="44"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="44"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
+      <c r="T10" s="44"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+      <c r="V10" s="44"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
+      <c r="X10" s="44"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+      <c r="Z10" s="44"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
@@ -1357,21 +1406,21 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="N11" s="44"/>
       <c r="O11" s="1">
         <v>1</v>
       </c>
-      <c r="P11" s="1"/>
+      <c r="P11" s="44"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="44"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="T11" s="44"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="V11" s="44"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
+      <c r="X11" s="44"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="44"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
@@ -1405,21 +1454,21 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="44"/>
       <c r="O12" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P12" s="1"/>
+      <c r="P12" s="44"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="R12" s="44"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="T12" s="44"/>
       <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="V12" s="44"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
+      <c r="X12" s="44"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="44"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
     </row>
@@ -1453,21 +1502,21 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="N13" s="44"/>
       <c r="O13" s="1">
         <v>1.2</v>
       </c>
-      <c r="P13" s="1"/>
+      <c r="P13" s="44"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="R13" s="44"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
+      <c r="T13" s="44"/>
       <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+      <c r="V13" s="44"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
+      <c r="X13" s="44"/>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Z13" s="44"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
     </row>
@@ -1501,21 +1550,21 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="N14" s="44"/>
       <c r="O14" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="44"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="R14" s="44"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+      <c r="T14" s="44"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+      <c r="V14" s="44"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
+      <c r="X14" s="44"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="44"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
@@ -1549,21 +1598,21 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="44"/>
       <c r="O15" s="1">
         <v>1.3</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="44"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="44"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
+      <c r="T15" s="44"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
+      <c r="V15" s="44"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
+      <c r="X15" s="44"/>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
+      <c r="Z15" s="44"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
@@ -1597,21 +1646,21 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="N16" s="44"/>
       <c r="O16" s="9">
         <v>1.3</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="P16" s="44"/>
       <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+      <c r="R16" s="44"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="T16" s="44"/>
       <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
+      <c r="V16" s="44"/>
       <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
+      <c r="X16" s="44"/>
       <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
+      <c r="Z16" s="44"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
     </row>
@@ -1645,21 +1694,21 @@
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="N17" s="44"/>
       <c r="O17" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P17" s="12"/>
+      <c r="P17" s="44"/>
       <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="R17" s="44"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
+      <c r="T17" s="44"/>
       <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
+      <c r="V17" s="44"/>
       <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
+      <c r="X17" s="44"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
+      <c r="Z17" s="44"/>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
     </row>
@@ -1693,21 +1742,21 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="N18" s="44"/>
       <c r="O18" s="13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P18" s="13"/>
+      <c r="P18" s="44"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
+      <c r="R18" s="44"/>
       <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
+      <c r="T18" s="44"/>
       <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
+      <c r="V18" s="44"/>
       <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
+      <c r="X18" s="44"/>
       <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
+      <c r="Z18" s="44"/>
       <c r="AA18" s="13"/>
       <c r="AB18" s="13"/>
     </row>
@@ -1741,21 +1790,21 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="N19" s="44"/>
       <c r="O19" s="13">
         <v>0.9</v>
       </c>
-      <c r="P19" s="13"/>
+      <c r="P19" s="44"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
+      <c r="R19" s="44"/>
       <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="T19" s="44"/>
       <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
+      <c r="V19" s="44"/>
       <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
+      <c r="X19" s="44"/>
       <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
+      <c r="Z19" s="44"/>
       <c r="AA19" s="13"/>
       <c r="AB19" s="13"/>
     </row>
@@ -1789,21 +1838,21 @@
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
+      <c r="N20" s="44"/>
       <c r="O20" s="18">
         <v>1.3</v>
       </c>
-      <c r="P20" s="18"/>
+      <c r="P20" s="44"/>
       <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
+      <c r="R20" s="44"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
+      <c r="T20" s="44"/>
       <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
+      <c r="V20" s="44"/>
       <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
+      <c r="X20" s="44"/>
       <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
+      <c r="Z20" s="44"/>
       <c r="AA20" s="18"/>
       <c r="AB20" s="18"/>
     </row>
@@ -1837,25 +1886,25 @@
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
+      <c r="N21" s="44"/>
       <c r="O21" s="23">
         <v>1.3</v>
       </c>
-      <c r="P21" s="23"/>
+      <c r="P21" s="44"/>
       <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
+      <c r="R21" s="44"/>
       <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
+      <c r="T21" s="44"/>
       <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
+      <c r="V21" s="44"/>
       <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
+      <c r="X21" s="44"/>
       <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
+      <c r="Z21" s="44"/>
       <c r="AA21" s="23"/>
       <c r="AB21" s="23"/>
       <c r="AD21" s="25" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1890,21 +1939,21 @@
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
       <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
+      <c r="N22" s="44"/>
       <c r="O22" s="26">
         <v>0.9</v>
       </c>
-      <c r="P22" s="26"/>
+      <c r="P22" s="44"/>
       <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
+      <c r="R22" s="44"/>
       <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
+      <c r="T22" s="44"/>
       <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
+      <c r="V22" s="44"/>
       <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
+      <c r="X22" s="44"/>
       <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
+      <c r="Z22" s="44"/>
       <c r="AA22" s="26"/>
       <c r="AB22" s="26"/>
     </row>
@@ -1938,73 +1987,73 @@
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
       <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
+      <c r="N23" s="44"/>
       <c r="O23" s="26">
         <v>1</v>
       </c>
-      <c r="P23" s="26"/>
+      <c r="P23" s="44"/>
       <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
+      <c r="R23" s="44"/>
       <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
+      <c r="T23" s="44"/>
       <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
+      <c r="V23" s="44"/>
       <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
+      <c r="X23" s="44"/>
       <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
+      <c r="Z23" s="44"/>
       <c r="AA23" s="26"/>
       <c r="AB23" s="26"/>
     </row>
-    <row r="24" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28">
-        <v>25</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="28" t="s">
+    <row r="24" spans="1:32" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30">
+        <v>25</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27">
+      <c r="F24" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="31">
         <v>1.4</v>
       </c>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-      <c r="V24" s="27"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
       <c r="AD24" s="28" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AE24" s="27">
         <v>23.5</v>
@@ -2013,8 +2062,115 @@
         <v>23.5</v>
       </c>
     </row>
+    <row r="25" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4">
+        <v>31</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="43"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="43"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+    </row>
+    <row r="26" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="46"/>
+      <c r="B26" s="46">
+        <v>31</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="48"/>
+      <c r="Q26" s="47">
+        <v>0.2</v>
+      </c>
+      <c r="R26" s="48"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="48"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="48"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="48"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="48"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AD26" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="G1:I2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
@@ -2029,14 +2185,6 @@
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="G1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Second-solo flight done on 22 June.
</commit_message>
<xml_diff>
--- a/log/My_Flying_Logbook.xlsx
+++ b/log/My_Flying_Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haoren/Documents/PA28/log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BE8701-4D80-4446-9963-03C006193C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBA8C50-F26C-C046-8BDB-6FCF6F3B4E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{634C8D91-949A-EA46-A557-4B6714D72E97}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="61">
   <si>
     <t>Month</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>June</t>
+  </si>
+  <si>
+    <t>Second Solo Flight</t>
+  </si>
+  <si>
+    <t>Pre-first-solo Check</t>
+  </si>
+  <si>
+    <t>Pre-second-solo Check</t>
   </si>
 </sst>
 </file>
@@ -376,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -498,6 +507,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,27 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,10 +859,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -869,52 +884,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="42" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="46" t="s">
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="44" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="44" t="s">
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="44"/>
+      <c r="AB1" s="42"/>
       <c r="AD1" s="28" t="s">
         <v>49</v>
       </c>
@@ -926,50 +941,50 @@
       </c>
     </row>
     <row r="2" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="44" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44" t="s">
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44" t="s">
+      <c r="R2" s="42"/>
+      <c r="S2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44" t="s">
+      <c r="T2" s="42"/>
+      <c r="U2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44" t="s">
+      <c r="V2" s="42"/>
+      <c r="W2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44" t="s">
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44" t="s">
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="44" t="s">
+      <c r="AB2" s="42" t="s">
         <v>19</v>
       </c>
     </row>
@@ -986,8 +1001,8 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="2" t="s">
         <v>30</v>
       </c>
@@ -997,9 +1012,9 @@
       <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
       <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1042,8 +1057,8 @@
       <c r="Z3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
     </row>
     <row r="4" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2089,7 +2104,7 @@
         <v>25</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>29</v>
@@ -2220,8 +2235,112 @@
       <c r="AA27" s="32"/>
       <c r="AB27" s="32"/>
     </row>
+    <row r="28" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4">
+        <v>22</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+    </row>
+    <row r="29" spans="1:32" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="40"/>
+      <c r="B29" s="40">
+        <v>22</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="R29" s="35"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="35"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="35"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="35"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="35"/>
+      <c r="AA29" s="41"/>
+      <c r="AB29" s="41"/>
+    </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="G1:I2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
@@ -2236,14 +2355,6 @@
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="G1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>